<commit_message>
CMM022 - Update template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリスト.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリスト.xlsx
@@ -1174,8 +1174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" workbookViewId="0">
-      <selection activeCell="I198" sqref="I198"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -1184,7 +1184,8 @@
     <col min="2" max="2" width="17.140625" style="8" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" style="8" customWidth="1"/>
     <col min="4" max="4" width="18.140625" style="8" customWidth="1"/>
-    <col min="5" max="16384" width="10.7109375" style="8"/>
+    <col min="5" max="6" width="11" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.7109375" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">

</xml_diff>

<commit_message>
CMM022 - fix bug #109962( Export excel chưa đúng dữ liệu có trong data)
</commit_message>
<xml_diff>
--- a/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリスト.xlsx
+++ b/nts.uk/uk.com/com.file/nts.uk.file.com.infra/src/main/resources/report/マスタリスト.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="12">
   <si>
     <t>JCM008</t>
   </si>
@@ -152,422 +152,12 @@
     <t>P</t>
     <phoneticPr fontId="1"/>
   </si>
-  <si>
-    <t>01</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>2018/12/06 14:15:57</t>
-  </si>
-  <si>
-    <t>【日時】</t>
-  </si>
-  <si>
-    <t>【種類】</t>
-  </si>
-  <si>
-    <t>【会社】</t>
-  </si>
-  <si>
-    <t>0001 日通システム株式会社</t>
-    <rPh sb="5" eb="7">
-      <t>ニッツウ</t>
-    </rPh>
-    <rPh sb="11" eb="15">
-      <t>カブシキガイシャ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>【sheet名】</t>
-    <rPh sb="6" eb="7">
-      <t>メイ</t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>マスタリスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>共通マスタコード</t>
-    <rPh sb="0" eb="2">
-      <t>キョウツウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>コード</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>名称</t>
-    <rPh sb="0" eb="1">
-      <t>メイ</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>ショウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>使用開始日</t>
-    <rPh sb="0" eb="2">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>カイシビ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>使用終了日</t>
-    <rPh sb="0" eb="2">
-      <t>シヨウ</t>
-    </rPh>
-    <rPh sb="2" eb="5">
-      <t>シュウリョウビ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>雇用形態</t>
-    <rPh sb="0" eb="2">
-      <t>コヨウ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ケイタイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>正社員</t>
-    <rPh sb="0" eb="3">
-      <t>セイシャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>2019/10/04</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>9999/12/31</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>表示順</t>
-    <rPh sb="0" eb="2">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ジュン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>02</t>
-  </si>
-  <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>04</t>
-  </si>
-  <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>09</t>
-  </si>
-  <si>
-    <t>一般職社員</t>
-    <rPh sb="0" eb="2">
-      <t>イッパン</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ショク</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>勤務地限定社員</t>
-    <rPh sb="0" eb="3">
-      <t>キンムチ</t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t>ゲンテイ</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>職種限定社員</t>
-    <rPh sb="0" eb="2">
-      <t>ショクシュ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ゲンテイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>勤務時間限定社員</t>
-    <rPh sb="0" eb="2">
-      <t>キンム</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ジカン</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>ゲンテイ</t>
-    </rPh>
-    <rPh sb="6" eb="8">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>身体障害社員</t>
-    <rPh sb="0" eb="2">
-      <t>シンタイ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショウガイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>知的障害社員</t>
-    <rPh sb="0" eb="2">
-      <t>チテキ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショウガイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>精神障害社員</t>
-    <rPh sb="0" eb="2">
-      <t>セイシン</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>ショウガイ</t>
-    </rPh>
-    <rPh sb="4" eb="6">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>準社員</t>
-    <rPh sb="0" eb="1">
-      <t>ジュン</t>
-    </rPh>
-    <rPh sb="1" eb="3">
-      <t>シャイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>フルタイムパート</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>パートタイマー</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アルバイト</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
-    <t>12</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>6</t>
-  </si>
-  <si>
-    <t>7</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>02</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>分類</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>分類1</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>分類2</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>分類3</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>分類4</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>分類5</t>
-    <rPh sb="0" eb="2">
-      <t>ブンルイ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>03</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>職位グループ</t>
-    <rPh sb="0" eb="1">
-      <t>ショク</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>イ</t>
-    </rPh>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>役員</t>
-    <rPh sb="0" eb="2">
-      <t>ヤクイン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>本部長格</t>
-    <rPh sb="0" eb="3">
-      <t>ホンブチョウ</t>
-    </rPh>
-    <rPh sb="3" eb="4">
-      <t>カク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>部長格</t>
-    <rPh sb="0" eb="1">
-      <t>ブ</t>
-    </rPh>
-    <rPh sb="1" eb="2">
-      <t>チョウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>課長格</t>
-    <rPh sb="0" eb="2">
-      <t>カチョウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>係長格</t>
-    <rPh sb="0" eb="2">
-      <t>カカリチョウ</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>カク</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>CMM0022 グループ会社共通マスタの登録</t>
-    <rPh sb="12" eb="14">
-      <t>カイシャ</t>
-    </rPh>
-    <rPh sb="14" eb="16">
-      <t>キョウツウ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,13 +231,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="ＭＳ ゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
     </font>
     <font>
       <sz val="10"/>
@@ -798,7 +381,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -819,35 +402,26 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="22" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="22" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="3" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="6" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1172,10 +746,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15"/>
@@ -1189,556 +763,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
+      <c r="A1" s="11"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="11"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="13"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="12"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="12"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="16"/>
-      <c r="B9" s="16"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="16"/>
-      <c r="G9" s="16"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="A10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="11" t="s">
-        <v>29</v>
-      </c>
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D11" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>30</v>
-      </c>
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="16"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
     <row r="12" spans="1:7">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G12" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F13" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" s="10"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="10"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="E18" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F18" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G18" s="19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E19" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G19" s="19" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
-      <c r="C20" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F20" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
-      <c r="C21" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F21" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="10"/>
-      <c r="B22" s="10"/>
-      <c r="C22" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F22" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G22" s="19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="B23" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D23" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F23" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G23" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
-      <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D25" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G25" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
-      <c r="A26" s="10"/>
-      <c r="B26" s="10"/>
-      <c r="C26" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="E26" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="10"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="E27" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G27" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
-      <c r="A28" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="B28" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E28" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G28" s="19" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
-      <c r="A29" s="10"/>
-      <c r="B29" s="10"/>
-      <c r="C29" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G29" s="19" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
-      <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
-      <c r="C30" s="15" t="s">
-        <v>32</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F30" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G30" s="19" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="D31" s="10" t="s">
-        <v>73</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
-      <c r="A32" s="10"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="D32" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>27</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="10"/>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="10"/>
-      <c r="F33" s="10"/>
-      <c r="G33" s="10"/>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="18"/>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-    </row>
-    <row r="35" spans="1:7">
-      <c r="A35" s="9"/>
-      <c r="B35" s="9"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="9"/>
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <ignoredErrors>
-    <ignoredError sqref="A11:G32" numberStoredAsText="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
 

</xml_diff>